<commit_message>
TILES implementation. Updated libraries list sheet and configuration & implementation files related to tiles. Though tiled view is loading, tile element pages are not loading in this CL. Hoping to make it in next CL :)
</commit_message>
<xml_diff>
--- a/EduWeb_master_/EduWeb_Info.xlsx
+++ b/EduWeb_master_/EduWeb_Info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Sl. No</t>
   </si>
@@ -47,6 +47,51 @@
   </si>
   <si>
     <t>Download Link</t>
+  </si>
+  <si>
+    <t>DEPENDENCY FOR</t>
+  </si>
+  <si>
+    <t>Struts2 &amp; jsp</t>
+  </si>
+  <si>
+    <t>struts2+Tiles</t>
+  </si>
+  <si>
+    <t>struts2-convention-plugin-2.2.1.jar</t>
+  </si>
+  <si>
+    <t>commons-beanutils-1.8.3.jar</t>
+  </si>
+  <si>
+    <t>commons-digester-1.8.jar</t>
+  </si>
+  <si>
+    <t>slf4j-api-1.5.6.jar</t>
+  </si>
+  <si>
+    <t>slf4j-simple-1.5.4.jar</t>
+  </si>
+  <si>
+    <t>struts2-tiles-plugin-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-api-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-compat-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-core-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-jsp-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-servlet-2.2.0.jar</t>
+  </si>
+  <si>
+    <t>tiles-template-2.2.0.jar</t>
   </si>
 </sst>
 </file>
@@ -70,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,8 +128,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -107,11 +158,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -124,6 +212,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,143 +516,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B11:B21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>